<commit_message>
Updating simple test spreadsheet to include column and row spanning.
</commit_message>
<xml_diff>
--- a/res/simple.xlsx
+++ b/res/simple.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Work/Workspace/Open/KHerGe/xlsx/res/test/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Work/Desktop/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="13">
   <si>
     <t>Number</t>
   </si>
@@ -123,6 +123,12 @@
   <si>
     <t>General</t>
   </si>
+  <si>
+    <t>Column Span</t>
+  </si>
+  <si>
+    <t>Row Span</t>
+  </si>
 </sst>
 </file>
 
@@ -130,7 +136,7 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="2">
     <numFmt numFmtId="8" formatCode="&quot;$&quot;#,##0.00_);[Red]\(&quot;$&quot;#,##0.00\)"/>
-    <numFmt numFmtId="167" formatCode="[$-409]m/d/yy\ h:mm\ AM/PM;@"/>
+    <numFmt numFmtId="164" formatCode="[$-409]m/d/yy\ h:mm\ AM/PM;@"/>
   </numFmts>
   <fonts count="4" x14ac:knownFonts="1">
     <font>
@@ -182,15 +188,21 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="18" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="8" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="12" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -468,10 +480,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I2"/>
+  <dimension ref="A1:I4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+      <selection activeCell="C3" sqref="C3:C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -542,7 +554,23 @@
         <v>0.5</v>
       </c>
     </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A3" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="B3" s="8"/>
+      <c r="C3" s="9" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="C4" s="9"/>
+    </row>
   </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="A3:B3"/>
+    <mergeCell ref="C3:C4"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>

</xml_diff>